<commit_message>
final commit for hw5
</commit_message>
<xml_diff>
--- a/HW5/Book1.xlsx
+++ b/HW5/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PersonalProjects\CAP5610\HW5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEB9964-7115-448E-BA80-621C70692BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FD4CDE-5DFB-4870-A733-D4F9502B2F63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5040" yWindow="6360" windowWidth="10830" windowHeight="8385" xr2:uid="{BCEA84E4-3902-4BA6-BFB3-7126D545174F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCEA84E4-3902-4BA6-BFB3-7126D545174F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,22 +71,22 @@
     <t>(Euclidean)</t>
   </si>
   <si>
-    <t>Centroids for 3</t>
-  </si>
-  <si>
-    <t>Centroids for 4</t>
-  </si>
-  <si>
-    <t>Centroids for 1 &amp; 2</t>
-  </si>
-  <si>
-    <t>Using Centroids for 1 &amp; 2</t>
-  </si>
-  <si>
-    <t>Using Centroids for 3</t>
-  </si>
-  <si>
-    <t>Using Centroids for 4</t>
+    <t>Initial centroids for 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Initial centroids for 3</t>
+  </si>
+  <si>
+    <t>Initial centroids for 4</t>
+  </si>
+  <si>
+    <t>Final Centroids for 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Final Centroids for 3</t>
+  </si>
+  <si>
+    <t>Final Centroids for 4</t>
   </si>
 </sst>
 </file>
@@ -119,14 +119,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -134,6 +126,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,22 +395,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -425,7 +419,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,7 +428,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -443,10 +437,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -766,7 +766,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
     <row r="3" spans="2:16" ht="51" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
       <c r="C3" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="5"/>
@@ -811,7 +811,7 @@
       <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="23" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -823,13 +823,13 @@
       <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="31" t="s">
+      <c r="N3" s="29" t="s">
         <v>6</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="29" t="s">
         <v>6</v>
       </c>
     </row>
@@ -857,15 +857,15 @@
         <f>ABS(G4-$C$4)+ABS(H4-$D$4)</f>
         <v>2</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="24">
         <f>ABS(G4-$C$5)+ABS(H4-$D$5)</f>
         <v>3</v>
       </c>
-      <c r="K4" s="30">
+      <c r="K4" s="28">
         <f>SQRT((POWER(G4-$C$4,2)+POWER(H4-$D$4,2)))</f>
         <v>1.4142135623730951</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="27">
         <f>SQRT(POWER(G4-$C$5,2)+POWER(H4-$D$5,2))</f>
         <v>2.2360679774997898</v>
       </c>
@@ -873,7 +873,7 @@
         <f>ABS(G4-$C$8)+ABS(H4-$D$8)</f>
         <v>2</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="30">
         <f>ABS(G4-$C$9)+ABS(H4-$D$9)</f>
         <v>7</v>
       </c>
@@ -881,7 +881,7 @@
         <f>ABS(G4-$C$12)+ABS(H4-$D$12)</f>
         <v>3</v>
       </c>
-      <c r="P4" s="34">
+      <c r="P4" s="32">
         <f>ABS(G4-$C$13)+ABS(H4-$D$13)</f>
         <v>4</v>
       </c>
@@ -910,15 +910,15 @@
         <f t="shared" ref="I5:I13" si="0">ABS(G5-$C$4)+ABS(H5-$D$4)</f>
         <v>3</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="25">
         <f t="shared" ref="J5:J13" si="1">ABS(G5-$C$5)+ABS(H5-$D$5)</f>
         <v>2</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="26">
         <f>SQRT((POWER(G5-$C$4,2)+POWER(H5-$D$4,2)))</f>
         <v>2.2360679774997898</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="28">
         <f t="shared" ref="L5:L13" si="2">SQRT(POWER(G5-$C$5,2)+POWER(H5-$D$5,2))</f>
         <v>2</v>
       </c>
@@ -926,7 +926,7 @@
         <f>ABS(G5-$C$8)+ABS(H5-$D$8)</f>
         <v>1</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="30">
         <f t="shared" ref="N5:N13" si="3">ABS(G5-$C$9)+ABS(H5-$D$9)</f>
         <v>6</v>
       </c>
@@ -934,7 +934,7 @@
         <f t="shared" ref="O5:O13" si="4">ABS(G5-$C$12)+ABS(H5-$D$12)</f>
         <v>2</v>
       </c>
-      <c r="P5" s="34">
+      <c r="P5" s="32">
         <f t="shared" ref="P5:P13" si="5">ABS(G5-$C$13)+ABS(H5-$D$13)</f>
         <v>5</v>
       </c>
@@ -954,15 +954,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="24">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="28">
         <f>SQRT((POWER(G6-$C$4,2)+POWER(H6-$D$4,2)))</f>
         <v>2.8284271247461903</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="27">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -970,7 +970,7 @@
         <f t="shared" ref="M5:M13" si="6">ABS(G6-$C$8)+ABS(H6-$D$8)</f>
         <v>6</v>
       </c>
-      <c r="N6" s="32">
+      <c r="N6" s="30">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -978,7 +978,7 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="P6" s="33">
+      <c r="P6" s="31">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
@@ -986,7 +986,7 @@
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="5"/>
@@ -1003,15 +1003,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="25">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="26">
         <f t="shared" ref="K5:K13" si="7">SQRT((POWER(G7-$C$4,2)+POWER(H7-$D$4,2)))</f>
         <v>3.6055512754639891</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="28">
         <f t="shared" si="2"/>
         <v>3.1622776601683795</v>
       </c>
@@ -1019,7 +1019,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="N7" s="32">
+      <c r="N7" s="30">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -1027,7 +1027,7 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="P7" s="34">
+      <c r="P7" s="32">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
@@ -1056,15 +1056,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="25">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="26">
         <f t="shared" si="7"/>
         <v>4.4721359549995796</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="28">
         <f t="shared" si="2"/>
         <v>2.2360679774997898</v>
       </c>
@@ -1072,7 +1072,7 @@
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="N8" s="33">
+      <c r="N8" s="31">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -1080,7 +1080,7 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="P8" s="34">
+      <c r="P8" s="32">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
@@ -1109,15 +1109,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="25">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="26">
         <f t="shared" si="7"/>
         <v>2.8284271247461903</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="28">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1125,7 +1125,7 @@
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="31">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -1133,7 +1133,7 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="P9" s="34">
+      <c r="P9" s="32">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
@@ -1153,15 +1153,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="25">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="26">
         <f t="shared" si="7"/>
         <v>4.2426406871192848</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="28">
         <f t="shared" si="2"/>
         <v>2.2360679774997898</v>
       </c>
@@ -1169,7 +1169,7 @@
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="31">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -1177,7 +1177,7 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="P10" s="34">
+      <c r="P10" s="32">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
@@ -1185,7 +1185,7 @@
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="5"/>
@@ -1202,15 +1202,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="25">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="26">
         <f t="shared" si="7"/>
         <v>3.6055512754639891</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="28">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -1218,7 +1218,7 @@
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="N11" s="33">
+      <c r="N11" s="31">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -1226,7 +1226,7 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="32">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
@@ -1254,15 +1254,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J12" s="27">
+      <c r="J12" s="25">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="26">
         <f t="shared" si="7"/>
         <v>4.1231056256176606</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="28">
         <f t="shared" si="2"/>
         <v>3.1622776601683795</v>
       </c>
@@ -1270,7 +1270,7 @@
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="31">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -1278,7 +1278,7 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="P12" s="33">
+      <c r="P12" s="31">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
@@ -1306,15 +1306,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="24">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="26">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="28">
         <f t="shared" si="2"/>
         <v>2.8284271247461903</v>
       </c>
@@ -1322,7 +1322,7 @@
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="31">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
@@ -1330,41 +1330,41 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="P13" s="33">
+      <c r="P13" s="31">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="18.75" x14ac:dyDescent="0.25">
       <c r="F15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="16"/>
-      <c r="H15" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="19">
+      <c r="H15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="34">
         <f>AVERAGE(G4,G6,G13)</f>
         <v>4</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="33">
         <f>AVERAGE(H4,H6,H13)</f>
         <v>6.333333333333333</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F16" s="23" t="s">
+    <row r="16" spans="2:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="F16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="20">
+      <c r="G16" s="22"/>
+      <c r="H16" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="33">
         <f>AVERAGE(G5,G7,G8,G9,G10,G11,G12)</f>
         <v>5.5714285714285712</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="33">
         <f>AVERAGE(H5,H7,H8,H9,H10,H11,H12)</f>
         <v>3.5714285714285716</v>
       </c>
@@ -1375,36 +1375,36 @@
       </c>
       <c r="G17" s="18"/>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="F19" s="15" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="16"/>
-      <c r="H19" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="19">
+      <c r="H19" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="34">
         <f>AVERAGE(G4,G6)</f>
         <v>2.5</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="33">
         <f>AVERAGE(H4,H6)</f>
         <v>6.5</v>
       </c>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="23" t="s">
+    <row r="20" spans="6:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="F20" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="20">
+      <c r="G20" s="22"/>
+      <c r="H20" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="33">
         <f>AVERAGE(G5,G7,G8,G9,G10,G11,G12,G13)</f>
         <v>5.75</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="33">
         <f>AVERAGE(H5,H7,H8,H9,H10,H11,H12,H13)</f>
         <v>3.875</v>
       </c>
@@ -1415,36 +1415,36 @@
       </c>
       <c r="G21" s="18"/>
     </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="F23" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="16"/>
-      <c r="H23" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="19">
+      <c r="H23" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="34">
         <f>AVERAGE(G4,G5,G6,G7)</f>
         <v>2.5</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J23" s="33">
         <f>AVERAGE(H4,H5,H6,H7)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="23" t="s">
+    <row r="24" spans="6:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="F24" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="20">
+      <c r="G24" s="22"/>
+      <c r="H24" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="33">
         <f>AVERAGE(G8,G9,G10,G11,G12,G13)</f>
         <v>6.833333333333333</v>
       </c>
-      <c r="J24" s="20">
+      <c r="J24" s="33">
         <f>AVERAGE(H8,H9,H10,H11,H12,H13)</f>
         <v>4</v>
       </c>
@@ -1455,36 +1455,36 @@
       </c>
       <c r="G25" s="18"/>
     </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="F27" s="15" t="s">
         <v>17</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="19">
+      <c r="H27" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="34">
         <f>AVERAGE(G4,G5,G7,G8,G9,G10,G11)</f>
         <v>4.8571428571428568</v>
       </c>
-      <c r="J27" s="20">
+      <c r="J27" s="33">
         <f>AVERAGE(H4,H5,H7,H8,H9,H10,H11)</f>
         <v>3.5714285714285716</v>
       </c>
     </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F28" s="23" t="s">
+    <row r="28" spans="6:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="F28" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="20">
+      <c r="G28" s="22"/>
+      <c r="H28" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="33">
         <f>AVERAGE(G6,G12,G13)</f>
         <v>5.666666666666667</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J28" s="33">
         <f>AVERAGE(H6,H12,H13)</f>
         <v>6.333333333333333</v>
       </c>

</xml_diff>